<commit_message>
Auswertung Teil 1 und 2 fertig
</commit_message>
<xml_diff>
--- a/tables/s2.xlsx
+++ b/tables/s2.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="201" documentId="06A890951654D623D59CA55AD880F051F617C84A" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{A1FFA6F2-9BEC-4078-BCC4-D779B1C18EF2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geräteliste" sheetId="2" r:id="rId1"/>
@@ -13,6 +12,7 @@
     <sheet name="Messung2" sheetId="3" r:id="rId3"/>
     <sheet name="Messung3" sheetId="4" r:id="rId4"/>
     <sheet name="Messung4" sheetId="5" r:id="rId5"/>
+    <sheet name="Ergebnisse" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>Geräteliste</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Auswertung</t>
   </si>
   <si>
-    <t>$\Delta l_n$</t>
-  </si>
-  <si>
     <t>Lamba / cm</t>
   </si>
   <si>
@@ -99,6 +96,33 @@
   </si>
   <si>
     <t>rel. Abweichung</t>
+  </si>
+  <si>
+    <t>$\Delta l_1$</t>
+  </si>
+  <si>
+    <t>$\Delta l_2$</t>
+  </si>
+  <si>
+    <t>$\Delta l_3$</t>
+  </si>
+  <si>
+    <t>$\Delta l_4$</t>
+  </si>
+  <si>
+    <t>Messung</t>
+  </si>
+  <si>
+    <t>Frequenz</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Mittelwert Differenz</t>
+  </si>
+  <si>
+    <t>Lambda / cm</t>
   </si>
 </sst>
 </file>
@@ -485,7 +509,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:S6"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +564,7 @@
         <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -648,37 +672,37 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
         <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
       </c>
       <c r="P5" t="s">
         <v>12</v>
       </c>
       <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" t="s">
         <v>22</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <f>B2-B3</f>
         <v>92.5</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:K7" si="0">C2-C3</f>
+        <f t="shared" ref="C6:K6" si="0">C2-C3</f>
         <v>92.5</v>
       </c>
       <c r="D6">
@@ -714,7 +738,7 @@
         <v>92.7</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L4:L6" si="1">MEDIAN(B6:K6)</f>
+        <f t="shared" ref="L6" si="1">MEDIAN(B6:K6)</f>
         <v>92.55</v>
       </c>
       <c r="M6">
@@ -758,7 +782,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:S6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -918,30 +942,30 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
         <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
       </c>
       <c r="P5" t="s">
         <v>12</v>
       </c>
       <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" t="s">
         <v>22</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <f>B2-B3</f>
@@ -1027,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40C8743-F75E-451D-959A-C93FDF4A3F22}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1104,7 @@
         <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1188,30 +1212,30 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
         <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
       </c>
       <c r="P5" t="s">
         <v>12</v>
       </c>
       <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" t="s">
         <v>22</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <f>B2-B3</f>
@@ -1298,7 +1322,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:S6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1374,7 @@
         <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1458,30 +1482,30 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
         <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
       </c>
       <c r="P5" t="s">
         <v>12</v>
       </c>
       <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" t="s">
         <v>22</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <f>B2-B3</f>
@@ -1561,4 +1585,286 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A07E23B-0099-490C-A958-3CB1FE3D6FF9}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>Messung1!P2</f>
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <f>Messung1!M2</f>
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>Messung1!N2</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E2">
+        <f>Messung1!$O$2</f>
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>Messung1!$L$6</f>
+        <v>92.55</v>
+      </c>
+      <c r="G2">
+        <f>Messung1!M6</f>
+        <v>61.699999999999996</v>
+      </c>
+      <c r="H2">
+        <f>Messung1!N6</f>
+        <v>308.5</v>
+      </c>
+      <c r="I2">
+        <f>Messung1!O6</f>
+        <v>308.47369430820203</v>
+      </c>
+      <c r="J2">
+        <f>Messung1!P6</f>
+        <v>308.48684715410104</v>
+      </c>
+      <c r="K2">
+        <f>Messung1!Q6</f>
+        <v>343.14</v>
+      </c>
+      <c r="L2">
+        <f>Messung1!R6</f>
+        <v>-34.653152845898944</v>
+      </c>
+      <c r="M2">
+        <f>Messung1!S6</f>
+        <v>-10.098838038671953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>Messung2!$P$2</f>
+        <v>1000</v>
+      </c>
+      <c r="C3">
+        <f>Messung2!$M$2</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D3">
+        <f>Messung2!N2</f>
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <f>Messung2!O2</f>
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f>Messung2!L6</f>
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G3">
+        <f>Messung2!M6</f>
+        <v>33.950000000000003</v>
+      </c>
+      <c r="H3">
+        <f>Messung2!N6</f>
+        <v>339.5</v>
+      </c>
+      <c r="I3">
+        <f>Messung2!O6</f>
+        <v>339.47105094857238</v>
+      </c>
+      <c r="J3">
+        <f>Messung2!P6</f>
+        <v>339.48552547428619</v>
+      </c>
+      <c r="K3">
+        <f>Messung2!Q6</f>
+        <v>343.14</v>
+      </c>
+      <c r="L3">
+        <f>Messung2!R6</f>
+        <v>-3.6544745257137947</v>
+      </c>
+      <c r="M3">
+        <f>Messung2!S6</f>
+        <v>-1.0650097702727179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>Messung3!$P$2</f>
+        <v>1510</v>
+      </c>
+      <c r="C4">
+        <f>Messung3!M2</f>
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f>Messung3!N2</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E4">
+        <f>Messung3!O2</f>
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <f>Messung3!L6</f>
+        <v>90.7</v>
+      </c>
+      <c r="G4">
+        <f>Messung3!M6</f>
+        <v>22.675000000000001</v>
+      </c>
+      <c r="H4">
+        <f>Messung3!N6</f>
+        <v>342.39249999999998</v>
+      </c>
+      <c r="I4">
+        <f>Messung3!O6</f>
+        <v>342.363304306065</v>
+      </c>
+      <c r="J4">
+        <f>Messung3!P6</f>
+        <v>342.37790215303249</v>
+      </c>
+      <c r="K4">
+        <f>Messung3!Q6</f>
+        <v>343.14</v>
+      </c>
+      <c r="L4">
+        <f>Messung3!R6</f>
+        <v>-0.76209784696749239</v>
+      </c>
+      <c r="M4">
+        <f>Messung3!S6</f>
+        <v>-0.22209531006804895</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>Messung4!$P$2</f>
+        <v>2000</v>
+      </c>
+      <c r="C5">
+        <f>Messung4!M2</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D5">
+        <f>Messung4!N2</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E5">
+        <f>Messung4!O2</f>
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <f>Messung4!L6</f>
+        <v>94.6</v>
+      </c>
+      <c r="G5">
+        <f>Messung4!M6</f>
+        <v>17.2</v>
+      </c>
+      <c r="H5">
+        <f>Messung4!N6</f>
+        <v>344</v>
+      </c>
+      <c r="I5">
+        <f>Messung4!O6</f>
+        <v>344</v>
+      </c>
+      <c r="J5">
+        <f>Messung4!P6</f>
+        <v>344</v>
+      </c>
+      <c r="K5">
+        <f>Messung4!Q6</f>
+        <v>343.14</v>
+      </c>
+      <c r="L5">
+        <f>Messung4!R6</f>
+        <v>0.86000000000001364</v>
+      </c>
+      <c r="M5">
+        <f>Messung4!S6</f>
+        <v>0.25062656641603454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>